<commit_message>
autre correction de coquille dans equivalence 34346bb8872e412783121562336fc894c3f2e787
</commit_message>
<xml_diff>
--- a/MappingPosologie/ig/PN13-FHIR-prescmed-medicationComp-conceptmap.xlsx
+++ b/MappingPosologie/ig/PN13-FHIR-prescmed-medicationComp-conceptmap.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-13T16:49:25+00:00</t>
+    <t>2024-11-13T17:25:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -99,7 +99,7 @@
     <t>Target</t>
   </si>
   <si>
-    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/FrMecicationCompound</t>
+    <t>https://hl7.fr/ig/fhir/medication/StructureDefinition/FrMedicationCompound</t>
   </si>
   <si>
     <t>Display</t>

</xml_diff>

<commit_message>
Fix issue mapping Medication ab77bff992840669d45583ae812eee5175aff7fe
</commit_message>
<xml_diff>
--- a/MappingPosologie/ig/PN13-FHIR-prescmed-medicationComp-conceptmap.xlsx
+++ b/MappingPosologie/ig/PN13-FHIR-prescmed-medicationComp-conceptmap.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-17T10:25:25+00:00</t>
+    <t>2024-11-17T10:38:58+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Medication.form.coding.code</t>
+  </si>
+  <si>
+    <t>related-to</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -437,9 +440,7 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="2">
-        <v>31</v>
-      </c>
+      <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" t="s" s="2">
         <v>32</v>
@@ -450,9 +451,7 @@
       <c r="E4" s="2"/>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="2">
-        <v>31</v>
-      </c>
+      <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" t="s" s="2">
         <v>32</v>
@@ -461,6 +460,17 @@
         <v>33</v>
       </c>
       <c r="E5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s" s="2">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>